<commit_message>
update 2019-11-26 xu Model test
2019/11/26 15:22
</commit_message>
<xml_diff>
--- a/沈阳鹏斓面辅料采购程序/0.沈阳鹏斓面辅料采购程序.xlsx
+++ b/沈阳鹏斓面辅料采购程序/0.沈阳鹏斓面辅料采购程序.xlsx
@@ -1965,6 +1965,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -1975,6 +1982,74 @@
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1995,57 +2070,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -2054,30 +2078,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -2181,6 +2181,60 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2199,49 +2253,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2253,25 +2265,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2289,31 +2295,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2331,37 +2349,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2660,6 +2660,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2671,21 +2686,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2750,10 +2750,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2762,133 +2762,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3450,8 +3450,8 @@
   <sheetPr/>
   <dimension ref="A2:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3770,8 +3770,8 @@
   <sheetPr/>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>